<commit_message>
complete doc by lhw
</commit_message>
<xml_diff>
--- a/doc/组48_讨论记录.xlsx
+++ b/doc/组48_讨论记录.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft\Desktop\eclipse\NBAAnalysis\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4290"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +75,22 @@
   </si>
   <si>
     <t>20分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定测试阶段分工</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>集体检查产物，最后整理，阶段总结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60分钟</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -489,6 +509,34 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>42080.395833333336</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>42083.770833333336</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete all the docs which is ready for submit by lhw
meanwhile fix a bug through comparing with others
</commit_message>
<xml_diff>
--- a/doc/组48_讨论记录.xlsx
+++ b/doc/组48_讨论记录.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft\Desktop\eclipse\NBAAnalysis\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\work2015\git\NBAAnalysis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,11 +86,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>集体检查产物，最后整理，阶段总结</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>60分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>集体检查产物，最后整理，阶段总结，正式轮换组长。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -531,10 +531,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>